<commit_message>
new experiments, data, analysis, camera ready
</commit_message>
<xml_diff>
--- a/Model/CogSciModel/test.xlsx
+++ b/Model/CogSciModel/test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20412"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4960" yWindow="440" windowWidth="25360" windowHeight="16020" tabRatio="500"/>
+    <workbookView xWindow="3440" yWindow="220" windowWidth="25360" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="7">
   <si>
     <t>ant</t>
   </si>
@@ -34,6 +34,12 @@
   </si>
   <si>
     <t>busy</t>
+  </si>
+  <si>
+    <t>buffao</t>
+  </si>
+  <si>
+    <t>wild</t>
   </si>
 </sst>
 </file>
@@ -82,8 +88,32 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="59">
+  <cellStyleXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -146,7 +176,7 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="59">
+  <cellStyles count="83">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -176,6 +206,18 @@
     <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -205,6 +247,18 @@
     <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -534,15 +588,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="I2" sqref="I2:I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:9">
       <c r="C1" t="s">
         <v>2</v>
       </c>
@@ -553,7 +607,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -572,8 +626,11 @@
       <c r="G2">
         <v>0.10249572799999999</v>
       </c>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="I2">
+        <v>0.127188041</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -592,8 +649,11 @@
       <c r="G3">
         <v>0.13085459499999999</v>
       </c>
-    </row>
-    <row r="4" spans="1:7">
+      <c r="I3">
+        <v>8.5787136E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -612,8 +672,11 @@
       <c r="G4">
         <v>6.4489336999999994E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:7">
+      <c r="I4">
+        <v>6.9772448000000001E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -632,8 +695,11 @@
       <c r="G5">
         <v>8.2338325000000004E-2</v>
       </c>
-    </row>
-    <row r="6" spans="1:7">
+      <c r="I5">
+        <v>6.0471832000000003E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -652,8 +718,11 @@
       <c r="G6">
         <v>0.14515263</v>
       </c>
-    </row>
-    <row r="7" spans="1:7">
+      <c r="I6">
+        <v>0.27471833699999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -672,8 +741,11 @@
       <c r="G7">
         <v>0.243447257</v>
       </c>
-    </row>
-    <row r="8" spans="1:7">
+      <c r="I7">
+        <v>0.15571164700000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -692,8 +764,11 @@
       <c r="G8">
         <v>0.101290226</v>
       </c>
-    </row>
-    <row r="9" spans="1:7">
+      <c r="I8">
+        <v>0.122877287</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -712,8 +787,11 @@
       <c r="G9">
         <v>0.12993190299999999</v>
       </c>
-    </row>
-    <row r="10" spans="1:7">
+      <c r="I9">
+        <v>0.10347327100000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="B10">
         <f>SUM(B2+B3+B6+B7)</f>
         <v>0.59111102900000001</v>
@@ -723,7 +801,7 @@
         <v>0.62195020999999995</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:9">
       <c r="C11" t="s">
         <v>2</v>
       </c>
@@ -734,7 +812,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:9">
       <c r="A12" t="s">
         <v>1</v>
       </c>
@@ -748,7 +826,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:9">
       <c r="A13" t="s">
         <v>1</v>
       </c>
@@ -762,7 +840,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:9">
       <c r="A14" t="s">
         <v>1</v>
       </c>
@@ -776,7 +854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:9">
       <c r="A15" t="s">
         <v>1</v>
       </c>
@@ -790,7 +868,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:9">
       <c r="A16" t="s">
         <v>1</v>
       </c>
@@ -844,6 +922,108 @@
       </c>
       <c r="E19">
         <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="C21" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>